<commit_message>
introduciong savings and change background color
</commit_message>
<xml_diff>
--- a/fluxo_caixa.xlsx
+++ b/fluxo_caixa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandremoreira/Documents/py_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40F33C11-A466-C84A-947A-974CF2C5C54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B84C02-6F4F-BC48-B969-42D6A42A9B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="59">
   <si>
     <t>Data</t>
   </si>
@@ -207,6 +207,15 @@
   </si>
   <si>
     <t>Transporte</t>
+  </si>
+  <si>
+    <t>Reserva de Emergência</t>
+  </si>
+  <si>
+    <t>Reserva</t>
+  </si>
+  <si>
+    <t>Savings</t>
   </si>
 </sst>
 </file>
@@ -561,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2864,6 +2873,354 @@
         <v>1</v>
       </c>
       <c r="I79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>45818</v>
+      </c>
+      <c r="B80" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" t="s">
+        <v>57</v>
+      </c>
+      <c r="D80" s="4">
+        <v>500</v>
+      </c>
+      <c r="E80" t="s">
+        <v>58</v>
+      </c>
+      <c r="F80" t="s">
+        <v>34</v>
+      </c>
+      <c r="G80" t="s">
+        <v>31</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
+        <v>45848</v>
+      </c>
+      <c r="B81" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" s="4">
+        <v>500</v>
+      </c>
+      <c r="E81" t="s">
+        <v>58</v>
+      </c>
+      <c r="F81" t="s">
+        <v>34</v>
+      </c>
+      <c r="G81" t="s">
+        <v>31</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
+        <v>45879</v>
+      </c>
+      <c r="B82" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" t="s">
+        <v>57</v>
+      </c>
+      <c r="D82" s="4">
+        <v>500</v>
+      </c>
+      <c r="E82" t="s">
+        <v>58</v>
+      </c>
+      <c r="F82" t="s">
+        <v>34</v>
+      </c>
+      <c r="G82" t="s">
+        <v>31</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="2">
+        <v>45910</v>
+      </c>
+      <c r="B83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83" t="s">
+        <v>57</v>
+      </c>
+      <c r="D83" s="4">
+        <v>500</v>
+      </c>
+      <c r="E83" t="s">
+        <v>58</v>
+      </c>
+      <c r="F83" t="s">
+        <v>34</v>
+      </c>
+      <c r="G83" t="s">
+        <v>31</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="2">
+        <v>45940</v>
+      </c>
+      <c r="B84" t="s">
+        <v>56</v>
+      </c>
+      <c r="C84" t="s">
+        <v>57</v>
+      </c>
+      <c r="D84" s="4">
+        <v>500</v>
+      </c>
+      <c r="E84" t="s">
+        <v>58</v>
+      </c>
+      <c r="F84" t="s">
+        <v>34</v>
+      </c>
+      <c r="G84" t="s">
+        <v>31</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="2">
+        <v>45971</v>
+      </c>
+      <c r="B85" t="s">
+        <v>56</v>
+      </c>
+      <c r="C85" t="s">
+        <v>57</v>
+      </c>
+      <c r="D85" s="4">
+        <v>500</v>
+      </c>
+      <c r="E85" t="s">
+        <v>58</v>
+      </c>
+      <c r="F85" t="s">
+        <v>34</v>
+      </c>
+      <c r="G85" t="s">
+        <v>31</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="2">
+        <v>46001</v>
+      </c>
+      <c r="B86" t="s">
+        <v>56</v>
+      </c>
+      <c r="C86" t="s">
+        <v>57</v>
+      </c>
+      <c r="D86" s="4">
+        <v>500</v>
+      </c>
+      <c r="E86" t="s">
+        <v>58</v>
+      </c>
+      <c r="F86" t="s">
+        <v>34</v>
+      </c>
+      <c r="G86" t="s">
+        <v>31</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="2">
+        <v>46032</v>
+      </c>
+      <c r="B87" t="s">
+        <v>56</v>
+      </c>
+      <c r="C87" t="s">
+        <v>57</v>
+      </c>
+      <c r="D87" s="4">
+        <v>500</v>
+      </c>
+      <c r="E87" t="s">
+        <v>58</v>
+      </c>
+      <c r="F87" t="s">
+        <v>34</v>
+      </c>
+      <c r="G87" t="s">
+        <v>31</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="2">
+        <v>46063</v>
+      </c>
+      <c r="B88" t="s">
+        <v>56</v>
+      </c>
+      <c r="C88" t="s">
+        <v>57</v>
+      </c>
+      <c r="D88" s="4">
+        <v>500</v>
+      </c>
+      <c r="E88" t="s">
+        <v>58</v>
+      </c>
+      <c r="F88" t="s">
+        <v>34</v>
+      </c>
+      <c r="G88" t="s">
+        <v>31</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="2">
+        <v>46091</v>
+      </c>
+      <c r="B89" t="s">
+        <v>56</v>
+      </c>
+      <c r="C89" t="s">
+        <v>57</v>
+      </c>
+      <c r="D89" s="4">
+        <v>500</v>
+      </c>
+      <c r="E89" t="s">
+        <v>58</v>
+      </c>
+      <c r="F89" t="s">
+        <v>34</v>
+      </c>
+      <c r="G89" t="s">
+        <v>31</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="2">
+        <v>46122</v>
+      </c>
+      <c r="B90" t="s">
+        <v>56</v>
+      </c>
+      <c r="C90" t="s">
+        <v>57</v>
+      </c>
+      <c r="D90" s="4">
+        <v>500</v>
+      </c>
+      <c r="E90" t="s">
+        <v>58</v>
+      </c>
+      <c r="F90" t="s">
+        <v>34</v>
+      </c>
+      <c r="G90" t="s">
+        <v>31</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="2">
+        <v>46152</v>
+      </c>
+      <c r="B91" t="s">
+        <v>56</v>
+      </c>
+      <c r="C91" t="s">
+        <v>57</v>
+      </c>
+      <c r="D91" s="4">
+        <v>500</v>
+      </c>
+      <c r="E91" t="s">
+        <v>58</v>
+      </c>
+      <c r="F91" t="s">
+        <v>34</v>
+      </c>
+      <c r="G91" t="s">
+        <v>31</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new filter by actual day
</commit_message>
<xml_diff>
--- a/fluxo_caixa.xlsx
+++ b/fluxo_caixa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandremoreira/Documents/py_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77126AE-A398-1549-8E52-6F86C1DBEF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12E1E17-329A-4441-81AE-19B809303819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="64">
   <si>
     <t>Data</t>
   </si>
@@ -222,6 +222,15 @@
   </si>
   <si>
     <t>Reembolso</t>
+  </si>
+  <si>
+    <t>Secagem Roupas</t>
+  </si>
+  <si>
+    <t>Serviços</t>
+  </si>
+  <si>
+    <t>Acessórios Deacthlon</t>
   </si>
 </sst>
 </file>
@@ -586,10 +595,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I83"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -659,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45848</v>
       </c>
@@ -688,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45879</v>
       </c>
@@ -717,7 +727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45910</v>
       </c>
@@ -746,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45940</v>
       </c>
@@ -775,7 +785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45971</v>
       </c>
@@ -804,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>46001</v>
       </c>
@@ -833,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>46032</v>
       </c>
@@ -862,7 +872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>46063</v>
       </c>
@@ -891,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>46091</v>
       </c>
@@ -920,7 +930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>46122</v>
       </c>
@@ -949,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>46152</v>
       </c>
@@ -1007,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>45856</v>
       </c>
@@ -1036,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>45887</v>
       </c>
@@ -1065,7 +1075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>45918</v>
       </c>
@@ -1094,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>45948</v>
       </c>
@@ -1123,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>45979</v>
       </c>
@@ -1152,7 +1162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>46009</v>
       </c>
@@ -1181,7 +1191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>46040</v>
       </c>
@@ -1210,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>46071</v>
       </c>
@@ -1239,7 +1249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>46099</v>
       </c>
@@ -1268,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>46130</v>
       </c>
@@ -1297,7 +1307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>46160</v>
       </c>
@@ -1355,7 +1365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>45848</v>
       </c>
@@ -1384,7 +1394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>45879</v>
       </c>
@@ -1413,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>45910</v>
       </c>
@@ -1442,7 +1452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>45940</v>
       </c>
@@ -1471,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>45971</v>
       </c>
@@ -1500,7 +1510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>46001</v>
       </c>
@@ -1529,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>46032</v>
       </c>
@@ -1558,7 +1568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>46063</v>
       </c>
@@ -1587,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>46091</v>
       </c>
@@ -1616,7 +1626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>46122</v>
       </c>
@@ -1645,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>46152</v>
       </c>
@@ -1703,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>45848</v>
       </c>
@@ -1732,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>45879</v>
       </c>
@@ -1761,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>45910</v>
       </c>
@@ -1790,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>45940</v>
       </c>
@@ -1819,7 +1829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>45971</v>
       </c>
@@ -1848,7 +1858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>46001</v>
       </c>
@@ -1877,7 +1887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>46032</v>
       </c>
@@ -1906,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>46063</v>
       </c>
@@ -1935,7 +1945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46091</v>
       </c>
@@ -1964,7 +1974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>46122</v>
       </c>
@@ -1993,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>46152</v>
       </c>
@@ -2051,7 +2061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>45848</v>
       </c>
@@ -2080,7 +2090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>45879</v>
       </c>
@@ -2109,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>45910</v>
       </c>
@@ -2138,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>45940</v>
       </c>
@@ -2167,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>45971</v>
       </c>
@@ -2196,7 +2206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>46001</v>
       </c>
@@ -2225,7 +2235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>46032</v>
       </c>
@@ -2254,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>46063</v>
       </c>
@@ -2283,7 +2293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>46091</v>
       </c>
@@ -2312,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>46122</v>
       </c>
@@ -2341,7 +2351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>46152</v>
       </c>
@@ -2399,7 +2409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>45882</v>
       </c>
@@ -2428,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>45848</v>
       </c>
@@ -2486,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>45848</v>
       </c>
@@ -2515,7 +2525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>45879</v>
       </c>
@@ -2544,7 +2554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>45910</v>
       </c>
@@ -2573,7 +2583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>45940</v>
       </c>
@@ -2602,7 +2612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>45971</v>
       </c>
@@ -2865,7 +2875,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>45826</v>
+        <v>45818</v>
       </c>
       <c r="B79" t="s">
         <v>22</v>
@@ -2874,7 +2884,7 @@
         <v>23</v>
       </c>
       <c r="D79" s="4">
-        <v>1800</v>
+        <v>1910</v>
       </c>
       <c r="E79" t="s">
         <v>19</v>
@@ -3008,8 +3018,72 @@
         <v>1</v>
       </c>
     </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="2">
+        <v>45818</v>
+      </c>
+      <c r="B84" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" t="s">
+        <v>62</v>
+      </c>
+      <c r="D84" s="4">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E84" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" t="s">
+        <v>34</v>
+      </c>
+      <c r="G84" t="s">
+        <v>31</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="2">
+        <v>45818</v>
+      </c>
+      <c r="B85" t="s">
+        <v>63</v>
+      </c>
+      <c r="C85" t="s">
+        <v>38</v>
+      </c>
+      <c r="D85" s="4">
+        <v>119.98</v>
+      </c>
+      <c r="E85" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" t="s">
+        <v>34</v>
+      </c>
+      <c r="G85" t="s">
+        <v>31</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I83" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:I83" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <dateGroupItem year="2025" month="6" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -3100,15 +3174,15 @@
       </c>
       <c r="C2" s="4">
         <f>SUMPRODUCT((LANCAMENTOS!$A$2:$A$987&gt;=EOMONTH($A2,-1)+1)*(LANCAMENTOS!$A$2:$A$987&lt;=EOMONTH($A2,0))*(LANCAMENTOS!$E$2:$E$987="Expense")*(LANCAMENTOS!$D$2:$D$987))</f>
-        <v>5844.21</v>
+        <v>6113.99</v>
       </c>
       <c r="D2" s="4">
         <f t="shared" ref="D2:D13" si="0">B2-C2</f>
-        <v>1755.29</v>
+        <v>1485.5100000000002</v>
       </c>
       <c r="E2" s="4">
         <f>PARAMS!$B$1+D2</f>
-        <v>1755.29</v>
+        <v>1485.5100000000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -3130,7 +3204,7 @@
       </c>
       <c r="E3" s="4">
         <f t="shared" ref="E3:E13" si="1">E2+D3</f>
-        <v>5165.1900000000005</v>
+        <v>4895.41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3152,7 +3226,7 @@
       </c>
       <c r="E4" s="4">
         <f t="shared" si="1"/>
-        <v>6097.09</v>
+        <v>5827.3099999999995</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -3174,7 +3248,7 @@
       </c>
       <c r="E5" s="4">
         <f t="shared" si="1"/>
-        <v>10256.99</v>
+        <v>9987.2099999999991</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -3196,7 +3270,7 @@
       </c>
       <c r="E6" s="4">
         <f t="shared" si="1"/>
-        <v>14416.89</v>
+        <v>14147.109999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3218,7 +3292,7 @@
       </c>
       <c r="E7" s="4">
         <f t="shared" si="1"/>
-        <v>18576.79</v>
+        <v>18307.009999999998</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -3240,7 +3314,7 @@
       </c>
       <c r="E8" s="4">
         <f t="shared" si="1"/>
-        <v>22886.29</v>
+        <v>22616.51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3262,7 +3336,7 @@
       </c>
       <c r="E9" s="4">
         <f t="shared" si="1"/>
-        <v>27195.79</v>
+        <v>26926.01</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -3284,7 +3358,7 @@
       </c>
       <c r="E10" s="4">
         <f t="shared" si="1"/>
-        <v>31505.29</v>
+        <v>31235.51</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -3306,7 +3380,7 @@
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>35814.79</v>
+        <v>35545.009999999995</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3328,7 +3402,7 @@
       </c>
       <c r="E12" s="4">
         <f t="shared" si="1"/>
-        <v>40124.29</v>
+        <v>39854.509999999995</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -3350,7 +3424,7 @@
       </c>
       <c r="E13" s="4">
         <f t="shared" si="1"/>
-        <v>44433.79</v>
+        <v>44164.009999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>